<commit_message>
unique ID for non-market rows and columns
</commit_message>
<xml_diff>
--- a/data-raw/metadata_uk_2010.xlsx
+++ b/data-raw/metadata_uk_2010.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/iotables/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:40009_{A687A7B1-47EF-4A63-9AF8-37F71A15DC91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4D745560-7895-41D7-BC84-78802BDEE769}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:40009_{A687A7B1-47EF-4A63-9AF8-37F71A15DC91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{8B170FE7-A372-4CA3-B7F0-31308C43E560}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="304">
   <si>
     <t>uk_row</t>
   </si>
@@ -878,6 +878,69 @@
   </si>
   <si>
     <t>Local government</t>
+  </si>
+  <si>
+    <t>NM_38</t>
+  </si>
+  <si>
+    <t>NM_59-60</t>
+  </si>
+  <si>
+    <t>NM_84</t>
+  </si>
+  <si>
+    <t>NM_85</t>
+  </si>
+  <si>
+    <t>NM_86</t>
+  </si>
+  <si>
+    <t>NM_87-88</t>
+  </si>
+  <si>
+    <t>NM_90</t>
+  </si>
+  <si>
+    <t>NM_91</t>
+  </si>
+  <si>
+    <t>NM_93</t>
+  </si>
+  <si>
+    <t>NPISH_72</t>
+  </si>
+  <si>
+    <t>NPISH_74</t>
+  </si>
+  <si>
+    <t>NPISH_75</t>
+  </si>
+  <si>
+    <t>NPISH_82</t>
+  </si>
+  <si>
+    <t>NPISH_85</t>
+  </si>
+  <si>
+    <t>NPISH_86</t>
+  </si>
+  <si>
+    <t>NPISH_87-88</t>
+  </si>
+  <si>
+    <t>NPISH_90</t>
+  </si>
+  <si>
+    <t>NPISH_91</t>
+  </si>
+  <si>
+    <t>NPISH_93</t>
+  </si>
+  <si>
+    <t>NPISH_94</t>
+  </si>
+  <si>
+    <t>NPISH_96</t>
   </si>
 </sst>
 </file>
@@ -1754,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E238" workbookViewId="0">
-      <selection activeCell="E243" sqref="E243"/>
+    <sheetView tabSelected="1" topLeftCell="E236" workbookViewId="0">
+      <selection activeCell="M242" sqref="M242:M262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5098,8 +5161,8 @@
       <c r="A108" t="s">
         <v>251</v>
       </c>
-      <c r="B108" s="3">
-        <v>38</v>
+      <c r="B108" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="D108" t="s">
         <v>128</v>
@@ -5117,9 +5180,8 @@
         <f t="shared" si="2"/>
         <v>12001</v>
       </c>
-      <c r="L108" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NM_", B108), ".", "_"), " &amp; ", "-")</f>
-        <v>NM_38</v>
+      <c r="L108" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -5127,7 +5189,7 @@
         <v>251</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>87</v>
+        <v>284</v>
       </c>
       <c r="D109" t="s">
         <v>129</v>
@@ -5145,17 +5207,16 @@
         <f t="shared" si="2"/>
         <v>12002</v>
       </c>
-      <c r="L109" t="str">
-        <f t="shared" ref="L109:L116" si="4">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NM_", B109), ".", "_"), " &amp; ", "-")</f>
-        <v>NM_59-60</v>
+      <c r="L109" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>251</v>
       </c>
-      <c r="B110" s="3">
-        <v>84</v>
+      <c r="B110" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="D110" t="s">
         <v>130</v>
@@ -5173,17 +5234,16 @@
         <f t="shared" si="2"/>
         <v>12003</v>
       </c>
-      <c r="L110" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_84</v>
+      <c r="L110" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>251</v>
       </c>
-      <c r="B111" s="3">
-        <v>85</v>
+      <c r="B111" s="3" t="s">
+        <v>286</v>
       </c>
       <c r="D111" t="s">
         <v>131</v>
@@ -5201,17 +5261,16 @@
         <f t="shared" si="2"/>
         <v>12004</v>
       </c>
-      <c r="L111" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_85</v>
+      <c r="L111" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>251</v>
       </c>
-      <c r="B112" s="3">
-        <v>86</v>
+      <c r="B112" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="D112" t="s">
         <v>132</v>
@@ -5229,9 +5288,8 @@
         <f t="shared" si="2"/>
         <v>12005</v>
       </c>
-      <c r="L112" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_86</v>
+      <c r="L112" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -5239,7 +5297,7 @@
         <v>251</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>118</v>
+        <v>288</v>
       </c>
       <c r="D113" t="s">
         <v>133</v>
@@ -5257,17 +5315,16 @@
         <f t="shared" si="2"/>
         <v>12006</v>
       </c>
-      <c r="L113" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_87-88</v>
+      <c r="L113" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>251</v>
       </c>
-      <c r="B114" s="3">
-        <v>90</v>
+      <c r="B114" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="D114" t="s">
         <v>134</v>
@@ -5285,17 +5342,16 @@
         <f t="shared" si="2"/>
         <v>12007</v>
       </c>
-      <c r="L114" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_90</v>
+      <c r="L114" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>251</v>
       </c>
-      <c r="B115" s="3">
-        <v>91</v>
+      <c r="B115" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="D115" t="s">
         <v>135</v>
@@ -5313,17 +5369,16 @@
         <f t="shared" si="2"/>
         <v>12008</v>
       </c>
-      <c r="L115" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_91</v>
+      <c r="L115" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>251</v>
       </c>
-      <c r="B116" s="3">
-        <v>93</v>
+      <c r="B116" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="D116" t="s">
         <v>136</v>
@@ -5341,17 +5396,16 @@
         <f t="shared" si="2"/>
         <v>12009</v>
       </c>
-      <c r="L116" t="str">
-        <f t="shared" si="4"/>
-        <v>NM_93</v>
+      <c r="L116" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>251</v>
       </c>
-      <c r="B117" s="3">
-        <v>72</v>
+      <c r="B117" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="D117" t="s">
         <v>137</v>
@@ -5369,17 +5423,16 @@
         <f t="shared" si="2"/>
         <v>12010</v>
       </c>
-      <c r="L117" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NPISH_", B117), ".", "_"), " &amp; ", "-")</f>
-        <v>NPISH_72</v>
+      <c r="L117" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>251</v>
       </c>
-      <c r="B118" s="3">
-        <v>74</v>
+      <c r="B118" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="D118" t="s">
         <v>138</v>
@@ -5397,17 +5450,16 @@
         <f t="shared" si="2"/>
         <v>12011</v>
       </c>
-      <c r="L118" t="str">
-        <f t="shared" ref="L118:L128" si="5">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NPISH_", B118), ".", "_"), " &amp; ", "-")</f>
-        <v>NPISH_74</v>
+      <c r="L118" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>251</v>
       </c>
-      <c r="B119" s="3">
-        <v>75</v>
+      <c r="B119" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="D119" t="s">
         <v>139</v>
@@ -5425,17 +5477,16 @@
         <f t="shared" si="2"/>
         <v>12012</v>
       </c>
-      <c r="L119" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_75</v>
+      <c r="L119" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>251</v>
       </c>
-      <c r="B120" s="3">
-        <v>82</v>
+      <c r="B120" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="D120" t="s">
         <v>140</v>
@@ -5453,17 +5504,16 @@
         <f t="shared" si="2"/>
         <v>12013</v>
       </c>
-      <c r="L120" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_82</v>
+      <c r="L120" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>251</v>
       </c>
-      <c r="B121" s="3">
-        <v>85</v>
+      <c r="B121" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="D121" t="s">
         <v>141</v>
@@ -5481,17 +5531,16 @@
         <f t="shared" si="2"/>
         <v>12014</v>
       </c>
-      <c r="L121" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_85</v>
+      <c r="L121" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>251</v>
       </c>
-      <c r="B122" s="3">
-        <v>86</v>
+      <c r="B122" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="D122" t="s">
         <v>142</v>
@@ -5509,9 +5558,8 @@
         <f t="shared" si="2"/>
         <v>12015</v>
       </c>
-      <c r="L122" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_86</v>
+      <c r="L122" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
@@ -5519,7 +5567,7 @@
         <v>251</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>118</v>
+        <v>298</v>
       </c>
       <c r="D123" t="s">
         <v>143</v>
@@ -5537,17 +5585,16 @@
         <f t="shared" si="2"/>
         <v>12016</v>
       </c>
-      <c r="L123" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_87-88</v>
+      <c r="L123" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>251</v>
       </c>
-      <c r="B124" s="3">
-        <v>90</v>
+      <c r="B124" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="D124" t="s">
         <v>144</v>
@@ -5565,17 +5612,16 @@
         <f t="shared" si="2"/>
         <v>12017</v>
       </c>
-      <c r="L124" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_90</v>
+      <c r="L124" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>251</v>
       </c>
-      <c r="B125" s="3">
-        <v>91</v>
+      <c r="B125" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="D125" t="s">
         <v>145</v>
@@ -5593,17 +5639,16 @@
         <f t="shared" si="2"/>
         <v>12018</v>
       </c>
-      <c r="L125" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_91</v>
+      <c r="L125" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>251</v>
       </c>
-      <c r="B126" s="3">
-        <v>93</v>
+      <c r="B126" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="D126" t="s">
         <v>146</v>
@@ -5621,17 +5666,16 @@
         <f t="shared" si="2"/>
         <v>12019</v>
       </c>
-      <c r="L126" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_93</v>
+      <c r="L126" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="3">
-        <v>94</v>
+      <c r="B127" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="D127" t="s">
         <v>147</v>
@@ -5649,17 +5693,16 @@
         <f t="shared" si="2"/>
         <v>12020</v>
       </c>
-      <c r="L127" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_94</v>
+      <c r="L127" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>251</v>
       </c>
-      <c r="B128" s="3">
-        <v>96</v>
+      <c r="B128" s="3" t="s">
+        <v>303</v>
       </c>
       <c r="D128" t="s">
         <v>148</v>
@@ -5677,9 +5720,8 @@
         <f t="shared" si="2"/>
         <v>12021</v>
       </c>
-      <c r="L128" t="str">
-        <f t="shared" si="5"/>
-        <v>NPISH_96</v>
+      <c r="L128" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5740,7 +5782,7 @@
         <v>13002</v>
       </c>
       <c r="L130" t="str">
-        <f t="shared" ref="L130:L135" si="6">F130</f>
+        <f t="shared" ref="L130:L135" si="4">F130</f>
         <v>P7</v>
       </c>
     </row>
@@ -5767,11 +5809,11 @@
         <v>3</v>
       </c>
       <c r="J131">
-        <f t="shared" ref="J131:J135" si="7">10000*G131+1000*H131+I131</f>
+        <f t="shared" ref="J131:J135" si="5">10000*G131+1000*H131+I131</f>
         <v>13003</v>
       </c>
       <c r="L131" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>D21X31</v>
       </c>
     </row>
@@ -5798,11 +5840,11 @@
         <v>4</v>
       </c>
       <c r="J132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13004</v>
       </c>
       <c r="L132" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>D29X39</v>
       </c>
     </row>
@@ -5829,11 +5871,11 @@
         <v>5</v>
       </c>
       <c r="J133">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13005</v>
       </c>
       <c r="L133" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>D1</v>
       </c>
     </row>
@@ -5860,11 +5902,11 @@
         <v>6</v>
       </c>
       <c r="J134">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13006</v>
       </c>
       <c r="L134" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>B2A3G</v>
       </c>
     </row>
@@ -5891,11 +5933,11 @@
         <v>7</v>
       </c>
       <c r="J135">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13007</v>
       </c>
       <c r="L135" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>P1</v>
       </c>
     </row>
@@ -5919,11 +5961,11 @@
         <v>1</v>
       </c>
       <c r="K136">
-        <f t="shared" ref="K136:K167" si="8">10000*G136+1000*H136+I136</f>
+        <f t="shared" ref="K136:K167" si="6">10000*G136+1000*H136+I136</f>
         <v>11001</v>
       </c>
       <c r="M136" t="str">
-        <f t="shared" ref="M136:M167" si="9">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C136), ".", "_"), " &amp; ", "-")</f>
+        <f t="shared" ref="M136:M167" si="7">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C136), ".", "_"), " &amp; ", "-")</f>
         <v>CPA_01</v>
       </c>
     </row>
@@ -5947,11 +5989,11 @@
         <v>2</v>
       </c>
       <c r="K137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11002</v>
       </c>
       <c r="M137" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_02</v>
       </c>
     </row>
@@ -5975,11 +6017,11 @@
         <v>3</v>
       </c>
       <c r="K138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11003</v>
       </c>
       <c r="M138" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_03</v>
       </c>
     </row>
@@ -6003,11 +6045,11 @@
         <v>4</v>
       </c>
       <c r="K139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11004</v>
       </c>
       <c r="M139" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_05</v>
       </c>
     </row>
@@ -6031,11 +6073,11 @@
         <v>5</v>
       </c>
       <c r="K140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11005</v>
       </c>
       <c r="M140" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_06-07</v>
       </c>
     </row>
@@ -6059,11 +6101,11 @@
         <v>6</v>
       </c>
       <c r="K141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11006</v>
       </c>
       <c r="M141" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_08</v>
       </c>
     </row>
@@ -6087,11 +6129,11 @@
         <v>7</v>
       </c>
       <c r="K142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11007</v>
       </c>
       <c r="M142" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_09</v>
       </c>
     </row>
@@ -6115,11 +6157,11 @@
         <v>8</v>
       </c>
       <c r="K143">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11008</v>
       </c>
       <c r="M143" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_1</v>
       </c>
     </row>
@@ -6143,11 +6185,11 @@
         <v>9</v>
       </c>
       <c r="K144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11009</v>
       </c>
       <c r="M144" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_2-3</v>
       </c>
     </row>
@@ -6171,11 +6213,11 @@
         <v>10</v>
       </c>
       <c r="K145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11010</v>
       </c>
       <c r="M145" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_4</v>
       </c>
     </row>
@@ -6199,11 +6241,11 @@
         <v>11</v>
       </c>
       <c r="K146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11011</v>
       </c>
       <c r="M146" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_5</v>
       </c>
     </row>
@@ -6227,11 +6269,11 @@
         <v>12</v>
       </c>
       <c r="K147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11012</v>
       </c>
       <c r="M147" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_6</v>
       </c>
     </row>
@@ -6255,11 +6297,11 @@
         <v>13</v>
       </c>
       <c r="K148">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11013</v>
       </c>
       <c r="M148" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_7</v>
       </c>
     </row>
@@ -6283,11 +6325,11 @@
         <v>14</v>
       </c>
       <c r="K149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11014</v>
       </c>
       <c r="M149" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_8</v>
       </c>
     </row>
@@ -6311,11 +6353,11 @@
         <v>15</v>
       </c>
       <c r="K150">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11015</v>
       </c>
       <c r="M150" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_10_9</v>
       </c>
     </row>
@@ -6339,11 +6381,11 @@
         <v>16</v>
       </c>
       <c r="K151">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11016</v>
       </c>
       <c r="M151" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_11_01-6</v>
       </c>
     </row>
@@ -6367,11 +6409,11 @@
         <v>17</v>
       </c>
       <c r="K152">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11017</v>
       </c>
       <c r="M152" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_11_07</v>
       </c>
     </row>
@@ -6395,11 +6437,11 @@
         <v>18</v>
       </c>
       <c r="K153">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11018</v>
       </c>
       <c r="M153" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_12</v>
       </c>
     </row>
@@ -6423,11 +6465,11 @@
         <v>19</v>
       </c>
       <c r="K154">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11019</v>
       </c>
       <c r="M154" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_13</v>
       </c>
     </row>
@@ -6451,11 +6493,11 @@
         <v>20</v>
       </c>
       <c r="K155">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11020</v>
       </c>
       <c r="M155" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_14</v>
       </c>
     </row>
@@ -6479,11 +6521,11 @@
         <v>21</v>
       </c>
       <c r="K156">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11021</v>
       </c>
       <c r="M156" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_15</v>
       </c>
     </row>
@@ -6507,11 +6549,11 @@
         <v>22</v>
       </c>
       <c r="K157">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11022</v>
       </c>
       <c r="M157" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_16</v>
       </c>
     </row>
@@ -6535,11 +6577,11 @@
         <v>23</v>
       </c>
       <c r="K158">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11023</v>
       </c>
       <c r="M158" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_17</v>
       </c>
     </row>
@@ -6563,11 +6605,11 @@
         <v>24</v>
       </c>
       <c r="K159">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11024</v>
       </c>
       <c r="M159" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_18</v>
       </c>
     </row>
@@ -6591,11 +6633,11 @@
         <v>25</v>
       </c>
       <c r="K160">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11025</v>
       </c>
       <c r="M160" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_19</v>
       </c>
     </row>
@@ -6619,11 +6661,11 @@
         <v>26</v>
       </c>
       <c r="K161">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11026</v>
       </c>
       <c r="M161" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_20A</v>
       </c>
     </row>
@@ -6647,11 +6689,11 @@
         <v>27</v>
       </c>
       <c r="K162">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11027</v>
       </c>
       <c r="M162" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_20B</v>
       </c>
     </row>
@@ -6675,11 +6717,11 @@
         <v>28</v>
       </c>
       <c r="K163">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11028</v>
       </c>
       <c r="M163" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_20C</v>
       </c>
     </row>
@@ -6703,11 +6745,11 @@
         <v>29</v>
       </c>
       <c r="K164">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11029</v>
       </c>
       <c r="M164" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_20_3</v>
       </c>
     </row>
@@ -6731,11 +6773,11 @@
         <v>30</v>
       </c>
       <c r="K165">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11030</v>
       </c>
       <c r="M165" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_20-4</v>
       </c>
     </row>
@@ -6759,11 +6801,11 @@
         <v>31</v>
       </c>
       <c r="K166">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11031</v>
       </c>
       <c r="M166" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_20_5</v>
       </c>
     </row>
@@ -6787,11 +6829,11 @@
         <v>32</v>
       </c>
       <c r="K167">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11032</v>
       </c>
       <c r="M167" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>CPA_21</v>
       </c>
     </row>
@@ -6815,11 +6857,11 @@
         <v>33</v>
       </c>
       <c r="K168">
-        <f t="shared" ref="K168:K199" si="10">10000*G168+1000*H168+I168</f>
+        <f t="shared" ref="K168:K199" si="8">10000*G168+1000*H168+I168</f>
         <v>11033</v>
       </c>
       <c r="M168" t="str">
-        <f t="shared" ref="M168:M199" si="11">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C168), ".", "_"), " &amp; ", "-")</f>
+        <f t="shared" ref="M168:M199" si="9">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C168), ".", "_"), " &amp; ", "-")</f>
         <v>CPA_22</v>
       </c>
     </row>
@@ -6843,11 +6885,11 @@
         <v>34</v>
       </c>
       <c r="K169">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11034</v>
       </c>
       <c r="M169" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_23OTHER</v>
       </c>
     </row>
@@ -6871,11 +6913,11 @@
         <v>35</v>
       </c>
       <c r="K170">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11035</v>
       </c>
       <c r="M170" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_23-5-6</v>
       </c>
     </row>
@@ -6899,11 +6941,11 @@
         <v>36</v>
       </c>
       <c r="K171">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11036</v>
       </c>
       <c r="M171" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_24-1-3</v>
       </c>
     </row>
@@ -6927,11 +6969,11 @@
         <v>37</v>
       </c>
       <c r="K172">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11037</v>
       </c>
       <c r="M172" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_24-4-5</v>
       </c>
     </row>
@@ -6955,11 +6997,11 @@
         <v>38</v>
       </c>
       <c r="K173">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11038</v>
       </c>
       <c r="M173" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_25OTHER</v>
       </c>
     </row>
@@ -6983,11 +7025,11 @@
         <v>39</v>
       </c>
       <c r="K174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11039</v>
       </c>
       <c r="M174" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_25_4</v>
       </c>
     </row>
@@ -7011,11 +7053,11 @@
         <v>40</v>
       </c>
       <c r="K175">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11040</v>
       </c>
       <c r="M175" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_26</v>
       </c>
     </row>
@@ -7039,11 +7081,11 @@
         <v>41</v>
       </c>
       <c r="K176">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11041</v>
       </c>
       <c r="M176" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_27</v>
       </c>
     </row>
@@ -7067,11 +7109,11 @@
         <v>42</v>
       </c>
       <c r="K177">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11042</v>
       </c>
       <c r="M177" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_28</v>
       </c>
     </row>
@@ -7095,11 +7137,11 @@
         <v>43</v>
       </c>
       <c r="K178">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11043</v>
       </c>
       <c r="M178" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_29</v>
       </c>
     </row>
@@ -7123,11 +7165,11 @@
         <v>44</v>
       </c>
       <c r="K179">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11044</v>
       </c>
       <c r="M179" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_30_1</v>
       </c>
     </row>
@@ -7151,11 +7193,11 @@
         <v>45</v>
       </c>
       <c r="K180">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11045</v>
       </c>
       <c r="M180" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_30_3</v>
       </c>
     </row>
@@ -7179,11 +7221,11 @@
         <v>46</v>
       </c>
       <c r="K181">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11046</v>
       </c>
       <c r="M181" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_30OTHER</v>
       </c>
     </row>
@@ -7207,11 +7249,11 @@
         <v>47</v>
       </c>
       <c r="K182">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11047</v>
       </c>
       <c r="M182" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_31</v>
       </c>
     </row>
@@ -7235,11 +7277,11 @@
         <v>48</v>
       </c>
       <c r="K183">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11048</v>
       </c>
       <c r="M183" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_32</v>
       </c>
     </row>
@@ -7263,11 +7305,11 @@
         <v>49</v>
       </c>
       <c r="K184">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11049</v>
       </c>
       <c r="M184" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_33-15</v>
       </c>
     </row>
@@ -7291,11 +7333,11 @@
         <v>50</v>
       </c>
       <c r="K185">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11050</v>
       </c>
       <c r="M185" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_33-16</v>
       </c>
     </row>
@@ -7319,11 +7361,11 @@
         <v>51</v>
       </c>
       <c r="K186">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11051</v>
       </c>
       <c r="M186" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_33OTHER</v>
       </c>
     </row>
@@ -7347,11 +7389,11 @@
         <v>52</v>
       </c>
       <c r="K187">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11052</v>
       </c>
       <c r="M187" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_35-1</v>
       </c>
     </row>
@@ -7375,11 +7417,11 @@
         <v>53</v>
       </c>
       <c r="K188">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11053</v>
       </c>
       <c r="M188" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_35-2-3</v>
       </c>
     </row>
@@ -7403,11 +7445,11 @@
         <v>54</v>
       </c>
       <c r="K189">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11054</v>
       </c>
       <c r="M189" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_36</v>
       </c>
     </row>
@@ -7431,11 +7473,11 @@
         <v>55</v>
       </c>
       <c r="K190">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11055</v>
       </c>
       <c r="M190" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_37</v>
       </c>
     </row>
@@ -7459,11 +7501,11 @@
         <v>56</v>
       </c>
       <c r="K191">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11056</v>
       </c>
       <c r="M191" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_38</v>
       </c>
     </row>
@@ -7487,11 +7529,11 @@
         <v>57</v>
       </c>
       <c r="K192">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11057</v>
       </c>
       <c r="M192" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_39</v>
       </c>
     </row>
@@ -7515,11 +7557,11 @@
         <v>58</v>
       </c>
       <c r="K193">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11058</v>
       </c>
       <c r="M193" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_41-43</v>
       </c>
     </row>
@@ -7543,11 +7585,11 @@
         <v>59</v>
       </c>
       <c r="K194">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11059</v>
       </c>
       <c r="M194" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_45</v>
       </c>
     </row>
@@ -7571,11 +7613,11 @@
         <v>60</v>
       </c>
       <c r="K195">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11060</v>
       </c>
       <c r="M195" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_46</v>
       </c>
     </row>
@@ -7599,11 +7641,11 @@
         <v>61</v>
       </c>
       <c r="K196">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11061</v>
       </c>
       <c r="M196" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_47</v>
       </c>
     </row>
@@ -7627,11 +7669,11 @@
         <v>62</v>
       </c>
       <c r="K197">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11062</v>
       </c>
       <c r="M197" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_49_1-2</v>
       </c>
     </row>
@@ -7655,11 +7697,11 @@
         <v>63</v>
       </c>
       <c r="K198">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11063</v>
       </c>
       <c r="M198" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_49_3-5</v>
       </c>
     </row>
@@ -7683,11 +7725,11 @@
         <v>64</v>
       </c>
       <c r="K199">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>11064</v>
       </c>
       <c r="M199" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>CPA_50</v>
       </c>
     </row>
@@ -7711,11 +7753,11 @@
         <v>65</v>
       </c>
       <c r="K200">
-        <f t="shared" ref="K200:K231" si="12">10000*G200+1000*H200+I200</f>
+        <f t="shared" ref="K200:K231" si="10">10000*G200+1000*H200+I200</f>
         <v>11065</v>
       </c>
       <c r="M200" t="str">
-        <f t="shared" ref="M200:M231" si="13">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C200), ".", "_"), " &amp; ", "-")</f>
+        <f t="shared" ref="M200:M231" si="11">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C200), ".", "_"), " &amp; ", "-")</f>
         <v>CPA_51</v>
       </c>
     </row>
@@ -7739,11 +7781,11 @@
         <v>66</v>
       </c>
       <c r="K201">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11066</v>
       </c>
       <c r="M201" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_52</v>
       </c>
     </row>
@@ -7767,11 +7809,11 @@
         <v>67</v>
       </c>
       <c r="K202">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11067</v>
       </c>
       <c r="M202" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_53</v>
       </c>
     </row>
@@ -7795,11 +7837,11 @@
         <v>68</v>
       </c>
       <c r="K203">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11068</v>
       </c>
       <c r="M203" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_55</v>
       </c>
     </row>
@@ -7823,11 +7865,11 @@
         <v>69</v>
       </c>
       <c r="K204">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11069</v>
       </c>
       <c r="M204" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_56</v>
       </c>
     </row>
@@ -7851,11 +7893,11 @@
         <v>70</v>
       </c>
       <c r="K205">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11070</v>
       </c>
       <c r="M205" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_58</v>
       </c>
     </row>
@@ -7879,11 +7921,11 @@
         <v>71</v>
       </c>
       <c r="K206">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11071</v>
       </c>
       <c r="M206" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_59-60</v>
       </c>
     </row>
@@ -7907,11 +7949,11 @@
         <v>72</v>
       </c>
       <c r="K207">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11072</v>
       </c>
       <c r="M207" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_61</v>
       </c>
     </row>
@@ -7935,11 +7977,11 @@
         <v>73</v>
       </c>
       <c r="K208">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11073</v>
       </c>
       <c r="M208" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_62</v>
       </c>
     </row>
@@ -7963,11 +8005,11 @@
         <v>74</v>
       </c>
       <c r="K209">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11074</v>
       </c>
       <c r="M209" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_63</v>
       </c>
     </row>
@@ -7991,11 +8033,11 @@
         <v>75</v>
       </c>
       <c r="K210">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11075</v>
       </c>
       <c r="M210" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_64</v>
       </c>
     </row>
@@ -8019,11 +8061,11 @@
         <v>76</v>
       </c>
       <c r="K211">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11076</v>
       </c>
       <c r="M211" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_65_1-3</v>
       </c>
     </row>
@@ -8047,11 +8089,11 @@
         <v>77</v>
       </c>
       <c r="K212">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11077</v>
       </c>
       <c r="M212" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_66</v>
       </c>
     </row>
@@ -8075,11 +8117,11 @@
         <v>78</v>
       </c>
       <c r="K213">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11078</v>
       </c>
       <c r="M213" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_68_1-2</v>
       </c>
     </row>
@@ -8103,11 +8145,11 @@
         <v>79</v>
       </c>
       <c r="K214">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11079</v>
       </c>
       <c r="M214" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_68_2IMP</v>
       </c>
     </row>
@@ -8131,11 +8173,11 @@
         <v>80</v>
       </c>
       <c r="K215">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11080</v>
       </c>
       <c r="M215" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_68-3</v>
       </c>
     </row>
@@ -8159,11 +8201,11 @@
         <v>81</v>
       </c>
       <c r="K216">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11081</v>
       </c>
       <c r="M216" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_69-1</v>
       </c>
     </row>
@@ -8187,11 +8229,11 @@
         <v>82</v>
       </c>
       <c r="K217">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11082</v>
       </c>
       <c r="M217" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_69-2</v>
       </c>
     </row>
@@ -8215,11 +8257,11 @@
         <v>83</v>
       </c>
       <c r="K218">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11083</v>
       </c>
       <c r="M218" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_70</v>
       </c>
     </row>
@@ -8243,11 +8285,11 @@
         <v>84</v>
       </c>
       <c r="K219">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11084</v>
       </c>
       <c r="M219" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_71</v>
       </c>
     </row>
@@ -8271,11 +8313,11 @@
         <v>85</v>
       </c>
       <c r="K220">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11085</v>
       </c>
       <c r="M220" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_72</v>
       </c>
     </row>
@@ -8299,11 +8341,11 @@
         <v>86</v>
       </c>
       <c r="K221">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11086</v>
       </c>
       <c r="M221" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_73</v>
       </c>
     </row>
@@ -8327,11 +8369,11 @@
         <v>87</v>
       </c>
       <c r="K222">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11087</v>
       </c>
       <c r="M222" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_74</v>
       </c>
     </row>
@@ -8355,11 +8397,11 @@
         <v>88</v>
       </c>
       <c r="K223">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11088</v>
       </c>
       <c r="M223" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_75</v>
       </c>
     </row>
@@ -8383,11 +8425,11 @@
         <v>89</v>
       </c>
       <c r="K224">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11089</v>
       </c>
       <c r="M224" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_77</v>
       </c>
     </row>
@@ -8411,11 +8453,11 @@
         <v>90</v>
       </c>
       <c r="K225">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11090</v>
       </c>
       <c r="M225" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_78</v>
       </c>
     </row>
@@ -8439,11 +8481,11 @@
         <v>91</v>
       </c>
       <c r="K226">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11091</v>
       </c>
       <c r="M226" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_79</v>
       </c>
     </row>
@@ -8467,11 +8509,11 @@
         <v>92</v>
       </c>
       <c r="K227">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11092</v>
       </c>
       <c r="M227" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_80</v>
       </c>
     </row>
@@ -8495,11 +8537,11 @@
         <v>93</v>
       </c>
       <c r="K228">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11093</v>
       </c>
       <c r="M228" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_81</v>
       </c>
     </row>
@@ -8523,11 +8565,11 @@
         <v>94</v>
       </c>
       <c r="K229">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11094</v>
       </c>
       <c r="M229" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_82</v>
       </c>
     </row>
@@ -8551,11 +8593,11 @@
         <v>95</v>
       </c>
       <c r="K230">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11095</v>
       </c>
       <c r="M230" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_84</v>
       </c>
     </row>
@@ -8579,11 +8621,11 @@
         <v>96</v>
       </c>
       <c r="K231">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>11096</v>
       </c>
       <c r="M231" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>CPA_85</v>
       </c>
     </row>
@@ -8607,11 +8649,11 @@
         <v>97</v>
       </c>
       <c r="K232">
-        <f t="shared" ref="K232:K263" si="14">10000*G232+1000*H232+I232</f>
+        <f t="shared" ref="K232:K263" si="12">10000*G232+1000*H232+I232</f>
         <v>11097</v>
       </c>
       <c r="M232" t="str">
-        <f t="shared" ref="M232:M241" si="15">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C232), ".", "_"), " &amp; ", "-")</f>
+        <f t="shared" ref="M232:M241" si="13">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("CPA_", C232), ".", "_"), " &amp; ", "-")</f>
         <v>CPA_86</v>
       </c>
     </row>
@@ -8635,11 +8677,11 @@
         <v>98</v>
       </c>
       <c r="K233">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11098</v>
       </c>
       <c r="M233" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_87-88</v>
       </c>
     </row>
@@ -8663,11 +8705,11 @@
         <v>99</v>
       </c>
       <c r="K234">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11099</v>
       </c>
       <c r="M234" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_90</v>
       </c>
     </row>
@@ -8691,11 +8733,11 @@
         <v>100</v>
       </c>
       <c r="K235">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11100</v>
       </c>
       <c r="M235" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_91</v>
       </c>
     </row>
@@ -8719,11 +8761,11 @@
         <v>101</v>
       </c>
       <c r="K236">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11101</v>
       </c>
       <c r="M236" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_92</v>
       </c>
     </row>
@@ -8747,11 +8789,11 @@
         <v>102</v>
       </c>
       <c r="K237">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11102</v>
       </c>
       <c r="M237" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_93</v>
       </c>
     </row>
@@ -8775,11 +8817,11 @@
         <v>103</v>
       </c>
       <c r="K238">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11103</v>
       </c>
       <c r="M238" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_94</v>
       </c>
     </row>
@@ -8803,11 +8845,11 @@
         <v>104</v>
       </c>
       <c r="K239">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11104</v>
       </c>
       <c r="M239" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_95</v>
       </c>
     </row>
@@ -8831,11 +8873,11 @@
         <v>105</v>
       </c>
       <c r="K240">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11105</v>
       </c>
       <c r="M240" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_96</v>
       </c>
     </row>
@@ -8859,11 +8901,11 @@
         <v>106</v>
       </c>
       <c r="K241">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>11106</v>
       </c>
       <c r="M241" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>CPA_97</v>
       </c>
     </row>
@@ -8871,8 +8913,8 @@
       <c r="A242" t="s">
         <v>251</v>
       </c>
-      <c r="C242" s="3">
-        <v>38</v>
+      <c r="C242" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="E242" t="s">
         <v>128</v>
@@ -8887,12 +8929,11 @@
         <v>1</v>
       </c>
       <c r="K242">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12001</v>
       </c>
-      <c r="M242" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NM_", C242), ".", "_"), " &amp; ", "-")</f>
-        <v>NM_38</v>
+      <c r="M242" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.25">
@@ -8900,7 +8941,7 @@
         <v>251</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>87</v>
+        <v>284</v>
       </c>
       <c r="E243" t="s">
         <v>129</v>
@@ -8915,20 +8956,19 @@
         <v>2</v>
       </c>
       <c r="K243">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12002</v>
       </c>
-      <c r="M243" t="str">
-        <f t="shared" ref="M243:M250" si="16">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NM_", C243), ".", "_"), " &amp; ", "-")</f>
-        <v>NM_59-60</v>
+      <c r="M243" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>251</v>
       </c>
-      <c r="C244" s="3">
-        <v>84</v>
+      <c r="C244" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="E244" t="s">
         <v>130</v>
@@ -8943,20 +8983,19 @@
         <v>3</v>
       </c>
       <c r="K244">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12003</v>
       </c>
-      <c r="M244" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_84</v>
+      <c r="M244" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>251</v>
       </c>
-      <c r="C245" s="3">
-        <v>85</v>
+      <c r="C245" s="3" t="s">
+        <v>286</v>
       </c>
       <c r="E245" t="s">
         <v>131</v>
@@ -8971,20 +9010,19 @@
         <v>4</v>
       </c>
       <c r="K245">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12004</v>
       </c>
-      <c r="M245" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_85</v>
+      <c r="M245" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>251</v>
       </c>
-      <c r="C246" s="3">
-        <v>86</v>
+      <c r="C246" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="E246" t="s">
         <v>132</v>
@@ -8999,12 +9037,11 @@
         <v>5</v>
       </c>
       <c r="K246">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12005</v>
       </c>
-      <c r="M246" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_86</v>
+      <c r="M246" s="3" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="247" spans="1:13" x14ac:dyDescent="0.25">
@@ -9012,7 +9049,7 @@
         <v>251</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>118</v>
+        <v>288</v>
       </c>
       <c r="E247" t="s">
         <v>133</v>
@@ -9027,20 +9064,19 @@
         <v>6</v>
       </c>
       <c r="K247">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12006</v>
       </c>
-      <c r="M247" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_87-88</v>
+      <c r="M247" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>251</v>
       </c>
-      <c r="C248" s="3">
-        <v>90</v>
+      <c r="C248" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="E248" t="s">
         <v>134</v>
@@ -9055,20 +9091,19 @@
         <v>7</v>
       </c>
       <c r="K248">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12007</v>
       </c>
-      <c r="M248" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_90</v>
+      <c r="M248" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>251</v>
       </c>
-      <c r="C249" s="3">
-        <v>91</v>
+      <c r="C249" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="E249" t="s">
         <v>135</v>
@@ -9083,20 +9118,19 @@
         <v>8</v>
       </c>
       <c r="K249">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12008</v>
       </c>
-      <c r="M249" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_91</v>
+      <c r="M249" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>251</v>
       </c>
-      <c r="C250" s="3">
-        <v>93</v>
+      <c r="C250" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="E250" t="s">
         <v>136</v>
@@ -9111,20 +9145,19 @@
         <v>9</v>
       </c>
       <c r="K250">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12009</v>
       </c>
-      <c r="M250" t="str">
-        <f t="shared" si="16"/>
-        <v>NM_93</v>
+      <c r="M250" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>251</v>
       </c>
-      <c r="C251" s="3">
-        <v>72</v>
+      <c r="C251" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="E251" t="s">
         <v>137</v>
@@ -9139,20 +9172,19 @@
         <v>10</v>
       </c>
       <c r="K251">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12010</v>
       </c>
-      <c r="M251" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NPISH_", C251), ".", "_"), " &amp; ", "-")</f>
-        <v>NPISH_72</v>
+      <c r="M251" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
-      <c r="C252" s="3">
-        <v>74</v>
+      <c r="C252" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="E252" t="s">
         <v>138</v>
@@ -9167,20 +9199,19 @@
         <v>11</v>
       </c>
       <c r="K252">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12011</v>
       </c>
-      <c r="M252" t="str">
-        <f t="shared" ref="M252:M262" si="17">SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NPISH_", C252), ".", "_"), " &amp; ", "-")</f>
-        <v>NPISH_74</v>
+      <c r="M252" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>251</v>
       </c>
-      <c r="C253" s="3">
-        <v>75</v>
+      <c r="C253" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="E253" t="s">
         <v>139</v>
@@ -9195,20 +9226,19 @@
         <v>12</v>
       </c>
       <c r="K253">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12012</v>
       </c>
-      <c r="M253" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_75</v>
+      <c r="M253" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>251</v>
       </c>
-      <c r="C254" s="3">
-        <v>82</v>
+      <c r="C254" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="E254" t="s">
         <v>140</v>
@@ -9223,20 +9253,19 @@
         <v>13</v>
       </c>
       <c r="K254">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12013</v>
       </c>
-      <c r="M254" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_82</v>
+      <c r="M254" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>251</v>
       </c>
-      <c r="C255" s="3">
-        <v>85</v>
+      <c r="C255" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="E255" t="s">
         <v>141</v>
@@ -9251,20 +9280,19 @@
         <v>14</v>
       </c>
       <c r="K255">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12014</v>
       </c>
-      <c r="M255" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_85</v>
+      <c r="M255" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>251</v>
       </c>
-      <c r="C256" s="3">
-        <v>86</v>
+      <c r="C256" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="E256" t="s">
         <v>142</v>
@@ -9279,12 +9307,11 @@
         <v>15</v>
       </c>
       <c r="K256">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12015</v>
       </c>
-      <c r="M256" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_86</v>
+      <c r="M256" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
@@ -9292,7 +9319,7 @@
         <v>251</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>118</v>
+        <v>298</v>
       </c>
       <c r="E257" t="s">
         <v>143</v>
@@ -9307,20 +9334,19 @@
         <v>16</v>
       </c>
       <c r="K257">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12016</v>
       </c>
-      <c r="M257" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_87-88</v>
+      <c r="M257" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>251</v>
       </c>
-      <c r="C258" s="3">
-        <v>90</v>
+      <c r="C258" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="E258" t="s">
         <v>144</v>
@@ -9335,20 +9361,19 @@
         <v>17</v>
       </c>
       <c r="K258">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12017</v>
       </c>
-      <c r="M258" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_90</v>
+      <c r="M258" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>251</v>
       </c>
-      <c r="C259" s="3">
-        <v>91</v>
+      <c r="C259" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="E259" t="s">
         <v>145</v>
@@ -9363,20 +9388,19 @@
         <v>18</v>
       </c>
       <c r="K259">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12018</v>
       </c>
-      <c r="M259" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_91</v>
+      <c r="M259" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>251</v>
       </c>
-      <c r="C260" s="3">
-        <v>93</v>
+      <c r="C260" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="E260" t="s">
         <v>146</v>
@@ -9391,20 +9415,19 @@
         <v>19</v>
       </c>
       <c r="K260">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12019</v>
       </c>
-      <c r="M260" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_93</v>
+      <c r="M260" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>251</v>
       </c>
-      <c r="C261" s="3">
-        <v>94</v>
+      <c r="C261" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="E261" t="s">
         <v>147</v>
@@ -9419,20 +9442,19 @@
         <v>20</v>
       </c>
       <c r="K261">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12020</v>
       </c>
-      <c r="M261" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("NPISH_", C261), ".", "_"), " &amp; ", "-")</f>
-        <v>NPISH_94</v>
+      <c r="M261" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>251</v>
       </c>
-      <c r="C262" s="3">
-        <v>96</v>
+      <c r="C262" s="3" t="s">
+        <v>303</v>
       </c>
       <c r="E262" t="s">
         <v>148</v>
@@ -9447,12 +9469,11 @@
         <v>21</v>
       </c>
       <c r="K262">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>12021</v>
       </c>
-      <c r="M262" t="str">
-        <f t="shared" si="17"/>
-        <v>NPISH_96</v>
+      <c r="M262" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.25">
@@ -9475,7 +9496,7 @@
         <v>1</v>
       </c>
       <c r="K263">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>13001</v>
       </c>
       <c r="M263" t="s">
@@ -9502,7 +9523,7 @@
         <v>2</v>
       </c>
       <c r="K264">
-        <f t="shared" ref="K264:K273" si="18">10000*G264+1000*H264+I264</f>
+        <f t="shared" ref="K264:K273" si="14">10000*G264+1000*H264+I264</f>
         <v>13002</v>
       </c>
       <c r="M264" t="s">
@@ -9529,7 +9550,7 @@
         <v>3</v>
       </c>
       <c r="K265">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13003</v>
       </c>
       <c r="M265" t="s">
@@ -9556,7 +9577,7 @@
         <v>4</v>
       </c>
       <c r="K266">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13004</v>
       </c>
       <c r="M266" t="s">
@@ -9583,7 +9604,7 @@
         <v>5</v>
       </c>
       <c r="K267">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13005</v>
       </c>
       <c r="M267" t="s">
@@ -9610,7 +9631,7 @@
         <v>6</v>
       </c>
       <c r="K268">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13006</v>
       </c>
       <c r="M268" t="s">
@@ -9637,7 +9658,7 @@
         <v>7</v>
       </c>
       <c r="K269">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13007</v>
       </c>
       <c r="M269" t="s">
@@ -9664,7 +9685,7 @@
         <v>8</v>
       </c>
       <c r="K270">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13008</v>
       </c>
       <c r="M270" t="s">
@@ -9691,7 +9712,7 @@
         <v>9</v>
       </c>
       <c r="K271">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13009</v>
       </c>
       <c r="M271" t="s">
@@ -9718,7 +9739,7 @@
         <v>10</v>
       </c>
       <c r="K272">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>13010</v>
       </c>
       <c r="M272" t="s">
@@ -9745,7 +9766,7 @@
         <v>9</v>
       </c>
       <c r="K273">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>19009</v>
       </c>
       <c r="M273" t="s">

</xml_diff>